<commit_message>
American market persistency solved
</commit_message>
<xml_diff>
--- a/Results/American_market.xlsx
+++ b/Results/American_market.xlsx
@@ -502,7 +502,7 @@
         <v>0.01483</v>
       </c>
       <c r="D2" t="n">
-        <v>0.01483</v>
+        <v>0.008880000000000001</v>
       </c>
       <c r="E2" t="n">
         <v>0.01038</v>
@@ -522,7 +522,7 @@
         <v>0.02434</v>
       </c>
       <c r="D3" t="n">
-        <v>0.02434</v>
+        <v>0.04308</v>
       </c>
       <c r="E3" t="n">
         <v>0.03365</v>
@@ -542,7 +542,7 @@
         <v>0.64721</v>
       </c>
       <c r="D4" t="n">
-        <v>0.64721</v>
+        <v>0.98027</v>
       </c>
       <c r="E4" t="n">
         <v>0.80106</v>
@@ -566,7 +566,7 @@
         <v>0.01491</v>
       </c>
       <c r="D5" t="n">
-        <v>0.01491</v>
+        <v>0.00886</v>
       </c>
       <c r="E5" t="n">
         <v>0.0113</v>
@@ -586,7 +586,7 @@
         <v>0.01867</v>
       </c>
       <c r="D6" t="n">
-        <v>0.01867</v>
+        <v>0.04363</v>
       </c>
       <c r="E6" t="n">
         <v>0.03075</v>
@@ -606,7 +606,7 @@
         <v>0.39404</v>
       </c>
       <c r="D7" t="n">
-        <v>0.39404</v>
+        <v>0.99717</v>
       </c>
       <c r="E7" t="n">
         <v>0.75868</v>
@@ -630,7 +630,7 @@
         <v>0.01612</v>
       </c>
       <c r="D8" t="n">
-        <v>0.01612</v>
+        <v>0.01071</v>
       </c>
       <c r="E8" t="n">
         <v>0.01208</v>
@@ -650,7 +650,7 @@
         <v>0.02135</v>
       </c>
       <c r="D9" t="n">
-        <v>0.02135</v>
+        <v>0.03814</v>
       </c>
       <c r="E9" t="n">
         <v>0.04023</v>
@@ -670,7 +670,7 @@
         <v>0.53155</v>
       </c>
       <c r="D10" t="n">
-        <v>0.53155</v>
+        <v>1.01244</v>
       </c>
       <c r="E10" t="n">
         <v>1.27599</v>

</xml_diff>